<commit_message>
Updated with new info
</commit_message>
<xml_diff>
--- a/osiris/Documentation/STRBaseExtendedLocusList.xlsx
+++ b/osiris/Documentation/STRBaseExtendedLocusList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="77">
   <si>
     <t>Locus</t>
   </si>
@@ -234,6 +234,27 @@
   </si>
   <si>
     <t>MaxAllele</t>
+  </si>
+  <si>
+    <t>OsirisMin</t>
+  </si>
+  <si>
+    <t>OsirisMax</t>
+  </si>
+  <si>
+    <t>PP16</t>
+  </si>
+  <si>
+    <t>Kit</t>
+  </si>
+  <si>
+    <t>LadderMin</t>
+  </si>
+  <si>
+    <t>LadderMax</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -562,20 +583,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="7" width="8.88671875" style="2"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="10" width="8.88671875" style="2"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -585,8 +606,23 @@
       <c r="D1" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -596,8 +632,23 @@
       <c r="D2" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F2" s="2">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2">
+        <v>20</v>
+      </c>
+      <c r="I2" s="2">
+        <v>4</v>
+      </c>
+      <c r="J2" s="2">
+        <v>22</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -607,8 +658,23 @@
       <c r="D3" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F3" s="2">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2">
+        <v>15</v>
+      </c>
+      <c r="I3" s="2">
+        <v>2</v>
+      </c>
+      <c r="J3" s="2">
+        <v>18</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -618,8 +684,23 @@
       <c r="D4" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2">
+        <v>2</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>48</v>
       </c>
@@ -629,8 +710,23 @@
       <c r="D5" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F5" s="2">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2">
+        <v>13.3</v>
+      </c>
+      <c r="I5" s="2">
+        <v>3</v>
+      </c>
+      <c r="J5" s="2">
+        <v>15.1</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -640,8 +736,23 @@
       <c r="D6" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F6" s="2">
+        <v>6</v>
+      </c>
+      <c r="G6" s="2">
+        <v>13</v>
+      </c>
+      <c r="I6" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="J6" s="2">
+        <v>17.2</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -651,8 +762,23 @@
       <c r="D7" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F7" s="2">
+        <v>6</v>
+      </c>
+      <c r="G7" s="2">
+        <v>15</v>
+      </c>
+      <c r="I7" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="J7" s="2">
+        <v>19</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -662,8 +788,23 @@
       <c r="D8" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F8" s="2">
+        <v>6</v>
+      </c>
+      <c r="G8" s="2">
+        <v>14</v>
+      </c>
+      <c r="I8" s="2">
+        <v>5</v>
+      </c>
+      <c r="J8" s="2">
+        <v>18.2</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -673,8 +814,23 @@
       <c r="D9" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F9" s="2">
+        <v>10</v>
+      </c>
+      <c r="G9" s="2">
+        <v>22</v>
+      </c>
+      <c r="I9" s="2">
+        <v>7</v>
+      </c>
+      <c r="J9" s="2">
+        <v>26</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -684,8 +840,20 @@
       <c r="D10" s="2">
         <v>51.2</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F10" s="2">
+        <v>16</v>
+      </c>
+      <c r="G10" s="2">
+        <v>46.2</v>
+      </c>
+      <c r="I10" s="2">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="J10" s="2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -695,8 +863,23 @@
       <c r="D11" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F11" s="2">
+        <v>7</v>
+      </c>
+      <c r="G11" s="2">
+        <v>18</v>
+      </c>
+      <c r="I11" s="2">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2">
+        <v>20</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -706,8 +889,23 @@
       <c r="D12" s="2">
         <v>41.2</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F12" s="2">
+        <v>24</v>
+      </c>
+      <c r="G12" s="2">
+        <v>38</v>
+      </c>
+      <c r="I12" s="2">
+        <v>22.3</v>
+      </c>
+      <c r="J12" s="2">
+        <v>43</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -717,8 +915,23 @@
       <c r="D13" s="2">
         <v>28.3</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F13" s="2">
+        <v>8</v>
+      </c>
+      <c r="G13" s="2">
+        <v>27</v>
+      </c>
+      <c r="I13" s="2">
+        <v>2</v>
+      </c>
+      <c r="J13" s="2">
+        <v>29</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -728,8 +941,23 @@
       <c r="D14" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F14" s="2">
+        <v>7</v>
+      </c>
+      <c r="G14" s="2">
+        <v>16</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="J14" s="2">
+        <v>19</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -739,8 +967,23 @@
       <c r="D15" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F15" s="2">
+        <v>7</v>
+      </c>
+      <c r="G15" s="2">
+        <v>15</v>
+      </c>
+      <c r="I15" s="2">
+        <v>4</v>
+      </c>
+      <c r="J15" s="2">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -750,8 +993,23 @@
       <c r="D16" s="2">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F16" s="2">
+        <v>15</v>
+      </c>
+      <c r="G16" s="2">
+        <v>28</v>
+      </c>
+      <c r="I16" s="2">
+        <v>11</v>
+      </c>
+      <c r="J16" s="2">
+        <v>28</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -761,8 +1019,23 @@
       <c r="D17" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F17" s="2">
+        <v>9</v>
+      </c>
+      <c r="G17" s="2">
+        <v>17.2</v>
+      </c>
+      <c r="I17" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="J17" s="2">
+        <v>20</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -773,7 +1046,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -784,7 +1057,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -795,7 +1068,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -806,7 +1079,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -817,7 +1090,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -828,7 +1101,7 @@
         <v>39.200000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -838,8 +1111,23 @@
       <c r="D24" s="2">
         <v>26</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F24" s="2">
+        <v>5</v>
+      </c>
+      <c r="G24" s="2">
+        <v>24</v>
+      </c>
+      <c r="I24" s="2">
+        <v>2</v>
+      </c>
+      <c r="J24" s="2">
+        <v>42.3</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -849,8 +1137,23 @@
       <c r="D25" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F25" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G25" s="2">
+        <v>17</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="J25" s="2">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -861,7 +1164,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -872,17 +1175,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -893,7 +1196,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -904,7 +1207,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>

</xml_diff>